<commit_message>
Products import functionality & feature improvement
</commit_message>
<xml_diff>
--- a/public/fileStore/import_template/import_products_template.xlsx
+++ b/public/fileStore/import_template/import_products_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Little Pro\Desktop\APOTEk\APOTEK_SYSTEMS_POS\public\fileStore\import_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE0E323-A275-4781-9B44-0D8603733440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7419663E-12F7-46F0-AA78-FEC162F8AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E4D20C7-D269-441D-A8EC-D6C44E917C10}"/>
   </bookViews>
@@ -87,10 +87,10 @@
     </r>
   </si>
   <si>
-    <t>MEDICINE</t>
-  </si>
-  <si>
     <t>Mo cola</t>
+  </si>
+  <si>
+    <t>MEDICINES</t>
   </si>
 </sst>
 </file>
@@ -947,13 +947,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DEEFF03-B454-4866-8B40-EA869BDF4730}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.140625" customWidth="1"/>
@@ -994,16 +994,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100001</v>
+        <v>102048</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>

</xml_diff>